<commit_message>
- Login Form 구현 - Login Ajax API 정상 호출 확인
</commit_message>
<xml_diff>
--- a/vuejpa/Domain 구성.xlsx
+++ b/vuejpa/Domain 구성.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\study\vuejpa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA47BD76-3FED-418F-BF7F-61DB934E6142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C693FC59-2405-4F81-AF93-E912243EB33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,10 +95,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>유저의 등급 (일반유저, VIP, 어드민)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>유저의 이메일</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -136,6 +132,10 @@
   </si>
   <si>
     <t>설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저의 등급 (Silver, Gold, VIP, Admin)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -323,18 +323,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
@@ -352,6 +343,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,7 +636,7 @@
   <dimension ref="B2:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -648,17 +648,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="F2" s="2"/>
       <c r="H2" s="2"/>
@@ -669,16 +669,16 @@
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="2"/>
@@ -690,14 +690,14 @@
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="3"/>
-      <c r="C4" s="14" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="2"/>
@@ -709,14 +709,14 @@
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="3"/>
-      <c r="C5" s="14" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="2"/>
@@ -728,14 +728,14 @@
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="3"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="2"/>
@@ -747,15 +747,15 @@
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="3"/>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>17</v>
+      <c r="E7" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="F7" s="2"/>
       <c r="H7" s="2"/>
@@ -766,15 +766,15 @@
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="15" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>19</v>
+      <c r="E8" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="F8" s="2"/>
       <c r="H8" s="2"/>
@@ -785,15 +785,15 @@
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
-      <c r="C9" s="15" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>18</v>
+      <c r="E9" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="F9" s="2"/>
       <c r="H9" s="2"/>
@@ -804,15 +804,15 @@
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="3"/>
-      <c r="C10" s="15" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>20</v>
+      <c r="E10" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="F10" s="2"/>
       <c r="H10" s="2"/>
@@ -823,15 +823,15 @@
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="3"/>
-      <c r="C11" s="15" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>21</v>
+      <c r="E11" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="F11" s="2"/>
       <c r="H11" s="2"/>
@@ -842,15 +842,15 @@
       <c r="M11" s="2"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="8"/>
-      <c r="C12" s="16" t="s">
+      <c r="B12" s="16"/>
+      <c r="C12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>22</v>
+      <c r="E12" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="F12" s="2"/>
       <c r="H12" s="2"/>

</xml_diff>